<commit_message>
Updated to fix sample PD53344d_hum which had failed coverage evennes threshold and was included in the analyses
</commit_message>
<xml_diff>
--- a/metadata/6633-_2729_3248_sample_pair-manifest_complete_final_calling_list.xlsx
+++ b/metadata/6633-_2729_3248_sample_pair-manifest_complete_final_calling_list.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10329"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mdc1/Documents/Projects/PDX_models_Latin_America/6633_PDX_models_Latin_America_WES/results/seq_qc_report/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mdc1/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E57D87E-4387-1F44-B816-5E4CB72B3117}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{106E60A3-5858-BE40-8AF7-32A2F3B9A6EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20" yWindow="500" windowWidth="51180" windowHeight="17000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4046,10 +4046,10 @@
   <dimension ref="A1:AS89"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D38" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I1" sqref="I1:I1048576"/>
+      <selection pane="bottomRight" activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9207,7 +9207,7 @@
         <v>270</v>
       </c>
       <c r="F45" t="s">
-        <v>1114</v>
+        <v>1116</v>
       </c>
       <c r="G45" s="4">
         <v>3248</v>

</xml_diff>